<commit_message>
Fix minor errors in data, mismatched plates, typos in Standard clone code
</commit_message>
<xml_diff>
--- a/data/RespirationRate/Block1_Day36_plate1_results_Oxygen.xlsx
+++ b/data/RespirationRate/Block1_Day36_plate1_results_Oxygen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PreSens\SDR_v4.0.0\Resource Quality Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/mlfearon_umich_edu/Documents/PROJECTS/MHMP Daphnia Duffy/Resource Quality/Data and Code/resource-quality-expt/data/RespirationRate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9ADF1E6-D7F3-442B-9A81-7DC2493ABB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{D9ADF1E6-D7F3-442B-9A81-7DC2493ABB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FB60BA0-A1DA-42CD-89F6-D6E181763278}"/>
   <bookViews>
-    <workbookView xWindow="4133" yWindow="3675" windowWidth="16875" windowHeight="10523" xr2:uid="{A18D23AB-8B16-4DB6-9AEF-25AFB3FB650E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A18D23AB-8B16-4DB6-9AEF-25AFB3FB650E}"/>
   </bookViews>
   <sheets>
     <sheet name="Oxygen Orginal" sheetId="2" r:id="rId1"/>
@@ -64,9 +64,6 @@
     <t>User Comment :</t>
   </si>
   <si>
-    <t>100% Scenedesmus</t>
-  </si>
-  <si>
     <t>Meas. Created By :</t>
   </si>
   <si>
@@ -464,6 +461,9 @@
   </si>
   <si>
     <t>14.12.21 11:48:38</t>
+  </si>
+  <si>
+    <t>50:50 Scenedesmus:Microcystis</t>
   </si>
 </sst>
 </file>
@@ -818,11 +818,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF32BBB0-92F1-4ABC-9847-7DC0770B2E08}">
   <dimension ref="A1:AF85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -836,22 +838,22 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -859,13 +861,13 @@
         <v>5</v>
       </c>
       <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -873,174 +875,174 @@
         <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3">
         <v>54.4</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I4">
         <v>46.95</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I5">
         <v>23.1</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I6">
         <v>23.1</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I7">
         <v>953</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="H8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>31</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>32</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>33</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>34</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>35</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>36</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>37</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>38</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>39</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>40</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>41</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>42</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>43</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>44</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>45</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>46</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>47</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>48</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
         <v>49</v>
       </c>
-      <c r="V13" t="s">
+      <c r="W13" t="s">
         <v>50</v>
       </c>
-      <c r="W13" t="s">
+      <c r="X13" t="s">
         <v>51</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Y13" t="s">
         <v>52</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="Z13" t="s">
         <v>53</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="AB13" t="s">
         <v>54</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AC13" t="s">
         <v>55</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AD13" t="s">
         <v>56</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AE13" t="s">
         <v>57</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AF13" t="s">
         <v>58</v>
       </c>
-      <c r="AF13" t="s">
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>60</v>
       </c>
       <c r="B14">
         <v>0.05</v>
@@ -1049,10 +1051,10 @@
         <v>121</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F14">
         <v>117.13</v>
@@ -1064,19 +1066,19 @@
         <v>119.99</v>
       </c>
       <c r="I14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J14">
         <v>118.64</v>
       </c>
       <c r="K14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L14">
         <v>116.96</v>
       </c>
       <c r="M14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N14">
         <v>116.46</v>
@@ -1097,13 +1099,13 @@
         <v>123.04</v>
       </c>
       <c r="T14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U14">
         <v>115.8</v>
       </c>
       <c r="V14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W14">
         <v>118.31</v>
@@ -1130,9 +1132,9 @@
         <v>21.75</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15">
         <v>2.0499999999999998</v>
@@ -1141,10 +1143,10 @@
         <v>119.99</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F15">
         <v>117.47</v>
@@ -1156,19 +1158,19 @@
         <v>118.98</v>
       </c>
       <c r="I15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J15">
         <v>117.8</v>
       </c>
       <c r="K15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L15">
         <v>116.13</v>
       </c>
       <c r="M15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N15">
         <v>115.96</v>
@@ -1189,13 +1191,13 @@
         <v>121.85</v>
       </c>
       <c r="T15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U15">
         <v>115.8</v>
       </c>
       <c r="V15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W15">
         <v>117.97</v>
@@ -1222,9 +1224,9 @@
         <v>21.79</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16">
         <v>4.07</v>
@@ -1233,10 +1235,10 @@
         <v>119.65</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F16">
         <v>117.3</v>
@@ -1248,19 +1250,19 @@
         <v>118.47</v>
       </c>
       <c r="I16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J16">
         <v>117.63</v>
       </c>
       <c r="K16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L16">
         <v>114.96</v>
       </c>
       <c r="M16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N16">
         <v>115.3</v>
@@ -1281,13 +1283,13 @@
         <v>120.66</v>
       </c>
       <c r="T16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U16">
         <v>115.96</v>
       </c>
       <c r="V16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W16">
         <v>117.63</v>
@@ -1314,9 +1316,9 @@
         <v>21.83</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17">
         <v>6.08</v>
@@ -1325,10 +1327,10 @@
         <v>118.98</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F17">
         <v>116.96</v>
@@ -1340,19 +1342,19 @@
         <v>117.8</v>
       </c>
       <c r="I17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J17">
         <v>116.46</v>
       </c>
       <c r="K17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L17">
         <v>114.46</v>
       </c>
       <c r="M17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N17">
         <v>114.96</v>
@@ -1373,13 +1375,13 @@
         <v>119.99</v>
       </c>
       <c r="T17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U17">
         <v>115.8</v>
       </c>
       <c r="V17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W17">
         <v>117.47</v>
@@ -1406,9 +1408,9 @@
         <v>21.84</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18">
         <v>8.1</v>
@@ -1417,10 +1419,10 @@
         <v>118.47</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F18">
         <v>116.8</v>
@@ -1432,19 +1434,19 @@
         <v>117.3</v>
       </c>
       <c r="I18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J18">
         <v>115.96</v>
       </c>
       <c r="K18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L18">
         <v>113.97</v>
       </c>
       <c r="M18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N18">
         <v>114.8</v>
@@ -1465,13 +1467,13 @@
         <v>118.98</v>
       </c>
       <c r="T18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U18">
         <v>115.96</v>
       </c>
       <c r="V18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W18">
         <v>117.3</v>
@@ -1498,9 +1500,9 @@
         <v>21.86</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B19">
         <v>10.1</v>
@@ -1509,10 +1511,10 @@
         <v>117.63</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F19">
         <v>116.63</v>
@@ -1524,19 +1526,19 @@
         <v>116.96</v>
       </c>
       <c r="I19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J19">
         <v>116.13</v>
       </c>
       <c r="K19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L19">
         <v>113.63</v>
       </c>
       <c r="M19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N19">
         <v>114.8</v>
@@ -1557,13 +1559,13 @@
         <v>117.8</v>
       </c>
       <c r="T19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U19">
         <v>115.63</v>
       </c>
       <c r="V19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W19">
         <v>117.3</v>
@@ -1590,9 +1592,9 @@
         <v>21.88</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20">
         <v>12.13</v>
@@ -1601,10 +1603,10 @@
         <v>117.13</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F20">
         <v>116.96</v>
@@ -1616,19 +1618,19 @@
         <v>116.96</v>
       </c>
       <c r="I20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J20">
         <v>116.46</v>
       </c>
       <c r="K20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L20">
         <v>113.63</v>
       </c>
       <c r="M20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N20">
         <v>114.46</v>
@@ -1649,13 +1651,13 @@
         <v>117.63</v>
       </c>
       <c r="T20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U20">
         <v>115.63</v>
       </c>
       <c r="V20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W20">
         <v>116.8</v>
@@ -1682,9 +1684,9 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B21">
         <v>14.13</v>
@@ -1693,10 +1695,10 @@
         <v>116.8</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F21">
         <v>116.96</v>
@@ -1708,19 +1710,19 @@
         <v>117.47</v>
       </c>
       <c r="I21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J21">
         <v>117.13</v>
       </c>
       <c r="K21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L21">
         <v>113.63</v>
       </c>
       <c r="M21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N21">
         <v>114.46</v>
@@ -1741,13 +1743,13 @@
         <v>117.47</v>
       </c>
       <c r="T21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U21">
         <v>115.3</v>
       </c>
       <c r="V21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W21">
         <v>116.96</v>
@@ -1774,9 +1776,9 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B22">
         <v>16.170000000000002</v>
@@ -1785,10 +1787,10 @@
         <v>116.3</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F22">
         <v>116.96</v>
@@ -1800,19 +1802,19 @@
         <v>117.47</v>
       </c>
       <c r="I22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J22">
         <v>117.47</v>
       </c>
       <c r="K22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L22">
         <v>113.97</v>
       </c>
       <c r="M22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N22">
         <v>114.8</v>
@@ -1833,13 +1835,13 @@
         <v>117.13</v>
       </c>
       <c r="T22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U22">
         <v>115.46</v>
       </c>
       <c r="V22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W22">
         <v>117.13</v>
@@ -1866,9 +1868,9 @@
         <v>21.88</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23">
         <v>18.18</v>
@@ -1877,10 +1879,10 @@
         <v>116.13</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F23">
         <v>116.8</v>
@@ -1892,19 +1894,19 @@
         <v>117.8</v>
       </c>
       <c r="I23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J23">
         <v>117.8</v>
       </c>
       <c r="K23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L23">
         <v>114.13</v>
       </c>
       <c r="M23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N23">
         <v>114.63</v>
@@ -1925,13 +1927,13 @@
         <v>116.63</v>
       </c>
       <c r="T23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U23">
         <v>115.63</v>
       </c>
       <c r="V23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W23">
         <v>117.13</v>
@@ -1958,9 +1960,9 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B24">
         <v>20.18</v>
@@ -1969,10 +1971,10 @@
         <v>116.13</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F24">
         <v>116.8</v>
@@ -1984,19 +1986,19 @@
         <v>117.47</v>
       </c>
       <c r="I24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J24">
         <v>117.3</v>
       </c>
       <c r="K24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L24">
         <v>114.13</v>
       </c>
       <c r="M24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N24">
         <v>114.46</v>
@@ -2017,13 +2019,13 @@
         <v>116.8</v>
       </c>
       <c r="T24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U24">
         <v>115.3</v>
       </c>
       <c r="V24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W24">
         <v>116.96</v>
@@ -2050,9 +2052,9 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B25">
         <v>22.18</v>
@@ -2061,10 +2063,10 @@
         <v>116.46</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F25">
         <v>116.8</v>
@@ -2076,19 +2078,19 @@
         <v>117.3</v>
       </c>
       <c r="I25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J25">
         <v>117.13</v>
       </c>
       <c r="K25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L25">
         <v>113.97</v>
       </c>
       <c r="M25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N25">
         <v>114.46</v>
@@ -2109,13 +2111,13 @@
         <v>116.46</v>
       </c>
       <c r="T25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U25">
         <v>115.3</v>
       </c>
       <c r="V25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W25">
         <v>116.8</v>
@@ -2142,9 +2144,9 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B26">
         <v>24.2</v>
@@ -2153,10 +2155,10 @@
         <v>116.13</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F26">
         <v>116.8</v>
@@ -2168,19 +2170,19 @@
         <v>117.13</v>
       </c>
       <c r="I26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J26">
         <v>117.3</v>
       </c>
       <c r="K26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L26">
         <v>113.63</v>
       </c>
       <c r="M26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N26">
         <v>114.13</v>
@@ -2201,13 +2203,13 @@
         <v>116.46</v>
       </c>
       <c r="T26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U26">
         <v>114.96</v>
       </c>
       <c r="V26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W26">
         <v>116.63</v>
@@ -2234,9 +2236,9 @@
         <v>21.88</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27">
         <v>26.2</v>
@@ -2245,10 +2247,10 @@
         <v>116.3</v>
       </c>
       <c r="D27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F27">
         <v>116.46</v>
@@ -2260,19 +2262,19 @@
         <v>116.8</v>
       </c>
       <c r="I27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J27">
         <v>117.3</v>
       </c>
       <c r="K27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L27">
         <v>113.63</v>
       </c>
       <c r="M27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N27">
         <v>113.97</v>
@@ -2293,13 +2295,13 @@
         <v>116.63</v>
       </c>
       <c r="T27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U27">
         <v>115.3</v>
       </c>
       <c r="V27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W27">
         <v>116.46</v>
@@ -2326,9 +2328,9 @@
         <v>21.88</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B28">
         <v>28.2</v>
@@ -2337,10 +2339,10 @@
         <v>116.63</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F28">
         <v>116.46</v>
@@ -2352,19 +2354,19 @@
         <v>116.63</v>
       </c>
       <c r="I28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J28">
         <v>116.96</v>
       </c>
       <c r="K28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L28">
         <v>113.63</v>
       </c>
       <c r="M28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N28">
         <v>113.47</v>
@@ -2385,13 +2387,13 @@
         <v>116.3</v>
       </c>
       <c r="T28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U28">
         <v>114.96</v>
       </c>
       <c r="V28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W28">
         <v>116.63</v>
@@ -2418,9 +2420,9 @@
         <v>21.88</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B29">
         <v>30.22</v>
@@ -2429,10 +2431,10 @@
         <v>116.63</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F29">
         <v>116.46</v>
@@ -2444,19 +2446,19 @@
         <v>116.3</v>
       </c>
       <c r="I29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J29">
         <v>116.8</v>
       </c>
       <c r="K29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L29">
         <v>113.8</v>
       </c>
       <c r="M29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N29">
         <v>113.97</v>
@@ -2477,13 +2479,13 @@
         <v>116.3</v>
       </c>
       <c r="T29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U29">
         <v>114.96</v>
       </c>
       <c r="V29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W29">
         <v>115.96</v>
@@ -2510,9 +2512,9 @@
         <v>21.86</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30">
         <v>32.22</v>
@@ -2521,10 +2523,10 @@
         <v>116.46</v>
       </c>
       <c r="D30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F30">
         <v>115.63</v>
@@ -2536,19 +2538,19 @@
         <v>115.63</v>
       </c>
       <c r="I30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J30">
         <v>116.46</v>
       </c>
       <c r="K30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L30">
         <v>113.47</v>
       </c>
       <c r="M30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N30">
         <v>113.63</v>
@@ -2569,13 +2571,13 @@
         <v>116.3</v>
       </c>
       <c r="T30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U30">
         <v>114.63</v>
       </c>
       <c r="V30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W30">
         <v>115.96</v>
@@ -2602,9 +2604,9 @@
         <v>21.86</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31">
         <v>34.22</v>
@@ -2613,10 +2615,10 @@
         <v>116.3</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F31">
         <v>116.13</v>
@@ -2628,19 +2630,19 @@
         <v>115.96</v>
       </c>
       <c r="I31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J31">
         <v>116.13</v>
       </c>
       <c r="K31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L31">
         <v>113.8</v>
       </c>
       <c r="M31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N31">
         <v>113.14</v>
@@ -2661,13 +2663,13 @@
         <v>115.96</v>
       </c>
       <c r="T31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U31">
         <v>114.63</v>
       </c>
       <c r="V31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W31">
         <v>115.96</v>
@@ -2694,9 +2696,9 @@
         <v>21.84</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B32">
         <v>36.22</v>
@@ -2705,10 +2707,10 @@
         <v>115.63</v>
       </c>
       <c r="D32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F32">
         <v>115.63</v>
@@ -2720,19 +2722,19 @@
         <v>115.46</v>
       </c>
       <c r="I32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J32">
         <v>115.8</v>
       </c>
       <c r="K32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L32">
         <v>113.47</v>
       </c>
       <c r="M32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N32">
         <v>113.3</v>
@@ -2753,13 +2755,13 @@
         <v>116.13</v>
       </c>
       <c r="T32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U32">
         <v>114.63</v>
       </c>
       <c r="V32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W32">
         <v>115.63</v>
@@ -2786,9 +2788,9 @@
         <v>21.84</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B33">
         <v>38.22</v>
@@ -2797,10 +2799,10 @@
         <v>115.96</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F33">
         <v>115.96</v>
@@ -2812,19 +2814,19 @@
         <v>115.13</v>
       </c>
       <c r="I33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J33">
         <v>115.96</v>
       </c>
       <c r="K33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L33">
         <v>113.8</v>
       </c>
       <c r="M33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N33">
         <v>112.97</v>
@@ -2845,13 +2847,13 @@
         <v>115.96</v>
       </c>
       <c r="T33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U33">
         <v>114.46</v>
       </c>
       <c r="V33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W33">
         <v>115.96</v>
@@ -2878,9 +2880,9 @@
         <v>21.84</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B34">
         <v>40.229999999999997</v>
@@ -2889,10 +2891,10 @@
         <v>115.96</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F34">
         <v>115.96</v>
@@ -2904,19 +2906,19 @@
         <v>115.3</v>
       </c>
       <c r="I34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J34">
         <v>115.8</v>
       </c>
       <c r="K34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L34">
         <v>112.97</v>
       </c>
       <c r="M34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N34">
         <v>112.97</v>
@@ -2937,13 +2939,13 @@
         <v>116.96</v>
       </c>
       <c r="T34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U34">
         <v>114.46</v>
       </c>
       <c r="V34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W34">
         <v>115.63</v>
@@ -2970,9 +2972,9 @@
         <v>21.84</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35">
         <v>42.23</v>
@@ -2981,10 +2983,10 @@
         <v>115.96</v>
       </c>
       <c r="D35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F35">
         <v>115.8</v>
@@ -2996,19 +2998,19 @@
         <v>115.3</v>
       </c>
       <c r="I35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J35">
         <v>115.8</v>
       </c>
       <c r="K35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L35">
         <v>112.81</v>
       </c>
       <c r="M35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N35">
         <v>112.31</v>
@@ -3029,13 +3031,13 @@
         <v>116.8</v>
       </c>
       <c r="T35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U35">
         <v>114.63</v>
       </c>
       <c r="V35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W35">
         <v>115.63</v>
@@ -3062,9 +3064,9 @@
         <v>21.84</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B36">
         <v>44.23</v>
@@ -3073,10 +3075,10 @@
         <v>115.8</v>
       </c>
       <c r="D36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F36">
         <v>115.46</v>
@@ -3088,19 +3090,19 @@
         <v>114.96</v>
       </c>
       <c r="I36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J36">
         <v>115.96</v>
       </c>
       <c r="K36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L36">
         <v>112.97</v>
       </c>
       <c r="M36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N36">
         <v>112.47</v>
@@ -3121,13 +3123,13 @@
         <v>116.3</v>
       </c>
       <c r="T36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U36">
         <v>114.3</v>
       </c>
       <c r="V36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W36">
         <v>115.3</v>
@@ -3154,9 +3156,9 @@
         <v>21.84</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B37">
         <v>46.23</v>
@@ -3165,10 +3167,10 @@
         <v>115.46</v>
       </c>
       <c r="D37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F37">
         <v>115.46</v>
@@ -3180,19 +3182,19 @@
         <v>114.8</v>
       </c>
       <c r="I37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J37">
         <v>115.8</v>
       </c>
       <c r="K37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L37">
         <v>112.64</v>
       </c>
       <c r="M37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N37">
         <v>111.98</v>
@@ -3213,13 +3215,13 @@
         <v>116.13</v>
       </c>
       <c r="T37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U37">
         <v>113.97</v>
       </c>
       <c r="V37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W37">
         <v>115.13</v>
@@ -3246,9 +3248,9 @@
         <v>21.81</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B38">
         <v>48.25</v>
@@ -3257,10 +3259,10 @@
         <v>115.13</v>
       </c>
       <c r="D38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F38">
         <v>115.13</v>
@@ -3272,19 +3274,19 @@
         <v>114.46</v>
       </c>
       <c r="I38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J38">
         <v>115.13</v>
       </c>
       <c r="K38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L38">
         <v>112.14</v>
       </c>
       <c r="M38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N38">
         <v>112.14</v>
@@ -3305,13 +3307,13 @@
         <v>115.46</v>
       </c>
       <c r="T38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U38">
         <v>113.8</v>
       </c>
       <c r="V38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W38">
         <v>114.8</v>
@@ -3338,9 +3340,9 @@
         <v>21.81</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B39">
         <v>50.25</v>
@@ -3349,10 +3351,10 @@
         <v>115.3</v>
       </c>
       <c r="D39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F39">
         <v>115.3</v>
@@ -3364,19 +3366,19 @@
         <v>114.3</v>
       </c>
       <c r="I39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J39">
         <v>115.13</v>
       </c>
       <c r="K39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L39">
         <v>112.31</v>
       </c>
       <c r="M39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N39">
         <v>111.81</v>
@@ -3397,13 +3399,13 @@
         <v>115.8</v>
       </c>
       <c r="T39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U39">
         <v>113.8</v>
       </c>
       <c r="V39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W39">
         <v>115.13</v>
@@ -3430,9 +3432,9 @@
         <v>21.81</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B40">
         <v>52.25</v>
@@ -3441,10 +3443,10 @@
         <v>115.13</v>
       </c>
       <c r="D40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F40">
         <v>115.3</v>
@@ -3456,19 +3458,19 @@
         <v>113.97</v>
       </c>
       <c r="I40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J40">
         <v>115.13</v>
       </c>
       <c r="K40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L40">
         <v>112.31</v>
       </c>
       <c r="M40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N40">
         <v>111.48</v>
@@ -3489,13 +3491,13 @@
         <v>115.46</v>
       </c>
       <c r="T40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U40">
         <v>113.8</v>
       </c>
       <c r="V40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W40">
         <v>114.96</v>
@@ -3522,9 +3524,9 @@
         <v>21.79</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41">
         <v>54.25</v>
@@ -3533,10 +3535,10 @@
         <v>114.96</v>
       </c>
       <c r="D41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F41">
         <v>115.3</v>
@@ -3548,19 +3550,19 @@
         <v>113.8</v>
       </c>
       <c r="I41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J41">
         <v>114.63</v>
       </c>
       <c r="K41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L41">
         <v>112.47</v>
       </c>
       <c r="M41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N41">
         <v>111.48</v>
@@ -3581,13 +3583,13 @@
         <v>115.13</v>
       </c>
       <c r="T41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U41">
         <v>113.47</v>
       </c>
       <c r="V41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W41">
         <v>114.96</v>
@@ -3614,9 +3616,9 @@
         <v>21.79</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B42">
         <v>56.27</v>
@@ -3625,10 +3627,10 @@
         <v>114.96</v>
       </c>
       <c r="D42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F42">
         <v>115.3</v>
@@ -3640,19 +3642,19 @@
         <v>113.8</v>
       </c>
       <c r="I42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J42">
         <v>114.63</v>
       </c>
       <c r="K42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L42">
         <v>112.14</v>
       </c>
       <c r="M42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N42">
         <v>111.32</v>
@@ -3673,13 +3675,13 @@
         <v>114.96</v>
       </c>
       <c r="T42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U42">
         <v>113.47</v>
       </c>
       <c r="V42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W42">
         <v>114.63</v>
@@ -3706,9 +3708,9 @@
         <v>21.79</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B43">
         <v>58.27</v>
@@ -3717,10 +3719,10 @@
         <v>114.8</v>
       </c>
       <c r="D43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F43">
         <v>115.13</v>
@@ -3732,19 +3734,19 @@
         <v>113.47</v>
       </c>
       <c r="I43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J43">
         <v>114.46</v>
       </c>
       <c r="K43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L43">
         <v>112.31</v>
       </c>
       <c r="M43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N43">
         <v>110.99</v>
@@ -3765,13 +3767,13 @@
         <v>114.96</v>
       </c>
       <c r="T43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U43">
         <v>113.47</v>
       </c>
       <c r="V43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W43">
         <v>114.8</v>
@@ -3798,9 +3800,9 @@
         <v>21.79</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B44">
         <v>60.27</v>
@@ -3809,10 +3811,10 @@
         <v>114.63</v>
       </c>
       <c r="D44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F44">
         <v>114.8</v>
@@ -3824,19 +3826,19 @@
         <v>113.47</v>
       </c>
       <c r="I44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J44">
         <v>114.13</v>
       </c>
       <c r="K44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L44">
         <v>112.31</v>
       </c>
       <c r="M44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N44">
         <v>110.83</v>
@@ -3857,13 +3859,13 @@
         <v>115.13</v>
       </c>
       <c r="T44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U44">
         <v>113.14</v>
       </c>
       <c r="V44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W44">
         <v>114.63</v>
@@ -3890,9 +3892,9 @@
         <v>21.79</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B45">
         <v>62.27</v>
@@ -3901,10 +3903,10 @@
         <v>114.3</v>
       </c>
       <c r="D45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F45">
         <v>114.46</v>
@@ -3916,19 +3918,19 @@
         <v>113.3</v>
       </c>
       <c r="I45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J45">
         <v>114.13</v>
       </c>
       <c r="K45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L45">
         <v>111.98</v>
       </c>
       <c r="M45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N45">
         <v>110.66</v>
@@ -3949,13 +3951,13 @@
         <v>114.96</v>
       </c>
       <c r="T45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U45">
         <v>112.97</v>
       </c>
       <c r="V45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W45">
         <v>114.3</v>
@@ -3982,9 +3984,9 @@
         <v>21.75</v>
       </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B46">
         <v>64.27</v>
@@ -3993,10 +3995,10 @@
         <v>114.13</v>
       </c>
       <c r="D46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F46">
         <v>114.3</v>
@@ -4008,19 +4010,19 @@
         <v>112.97</v>
       </c>
       <c r="I46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J46">
         <v>113.97</v>
       </c>
       <c r="K46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L46">
         <v>111.32</v>
       </c>
       <c r="M46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N46">
         <v>110.83</v>
@@ -4041,13 +4043,13 @@
         <v>114.96</v>
       </c>
       <c r="T46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U46">
         <v>112.81</v>
       </c>
       <c r="V46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W46">
         <v>114.46</v>
@@ -4074,9 +4076,9 @@
         <v>21.75</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B47">
         <v>66.28</v>
@@ -4085,10 +4087,10 @@
         <v>113.8</v>
       </c>
       <c r="D47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F47">
         <v>114.63</v>
@@ -4100,19 +4102,19 @@
         <v>112.97</v>
       </c>
       <c r="I47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J47">
         <v>113.47</v>
       </c>
       <c r="K47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L47">
         <v>111.16</v>
       </c>
       <c r="M47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N47">
         <v>110.33</v>
@@ -4133,13 +4135,13 @@
         <v>114.96</v>
       </c>
       <c r="T47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U47">
         <v>112.47</v>
       </c>
       <c r="V47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W47">
         <v>114.3</v>
@@ -4166,9 +4168,9 @@
         <v>21.75</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B48">
         <v>68.28</v>
@@ -4177,10 +4179,10 @@
         <v>113.63</v>
       </c>
       <c r="D48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F48">
         <v>114.3</v>
@@ -4192,19 +4194,19 @@
         <v>112.64</v>
       </c>
       <c r="I48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J48">
         <v>113.63</v>
       </c>
       <c r="K48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L48">
         <v>111.81</v>
       </c>
       <c r="M48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N48">
         <v>110.5</v>
@@ -4225,13 +4227,13 @@
         <v>114.46</v>
       </c>
       <c r="T48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U48">
         <v>112.64</v>
       </c>
       <c r="V48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W48">
         <v>114.13</v>
@@ -4258,9 +4260,9 @@
         <v>21.74</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B49">
         <v>70.28</v>
@@ -4269,10 +4271,10 @@
         <v>113.47</v>
       </c>
       <c r="D49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F49">
         <v>114.3</v>
@@ -4284,19 +4286,19 @@
         <v>112.64</v>
       </c>
       <c r="I49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J49">
         <v>113.3</v>
       </c>
       <c r="K49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L49">
         <v>111.48</v>
       </c>
       <c r="M49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N49">
         <v>110</v>
@@ -4317,13 +4319,13 @@
         <v>114.46</v>
       </c>
       <c r="T49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U49">
         <v>112.31</v>
       </c>
       <c r="V49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W49">
         <v>114.13</v>
@@ -4350,9 +4352,9 @@
         <v>21.74</v>
       </c>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B50">
         <v>72.28</v>
@@ -4361,10 +4363,10 @@
         <v>113.3</v>
       </c>
       <c r="D50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F50">
         <v>114.13</v>
@@ -4376,19 +4378,19 @@
         <v>112.31</v>
       </c>
       <c r="I50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J50">
         <v>113.3</v>
       </c>
       <c r="K50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L50">
         <v>110.99</v>
       </c>
       <c r="M50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N50">
         <v>109.68</v>
@@ -4409,13 +4411,13 @@
         <v>114.13</v>
       </c>
       <c r="T50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U50">
         <v>112.31</v>
       </c>
       <c r="V50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W50">
         <v>113.97</v>
@@ -4442,9 +4444,9 @@
         <v>21.73</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B51">
         <v>74.3</v>
@@ -4453,10 +4455,10 @@
         <v>113.63</v>
       </c>
       <c r="D51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F51">
         <v>114.13</v>
@@ -4468,19 +4470,19 @@
         <v>111.98</v>
       </c>
       <c r="I51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J51">
         <v>112.97</v>
       </c>
       <c r="K51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L51">
         <v>111.32</v>
       </c>
       <c r="M51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N51">
         <v>109.84</v>
@@ -4501,13 +4503,13 @@
         <v>114.46</v>
       </c>
       <c r="T51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U51">
         <v>112.14</v>
       </c>
       <c r="V51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W51">
         <v>113.8</v>
@@ -4534,9 +4536,9 @@
         <v>21.74</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B52">
         <v>76.3</v>
@@ -4545,10 +4547,10 @@
         <v>113.63</v>
       </c>
       <c r="D52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F52">
         <v>114.13</v>
@@ -4560,19 +4562,19 @@
         <v>111.98</v>
       </c>
       <c r="I52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J52">
         <v>112.97</v>
       </c>
       <c r="K52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L52">
         <v>111.16</v>
       </c>
       <c r="M52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N52">
         <v>109.68</v>
@@ -4593,13 +4595,13 @@
         <v>114.13</v>
       </c>
       <c r="T52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U52">
         <v>112.31</v>
       </c>
       <c r="V52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W52">
         <v>113.8</v>
@@ -4626,9 +4628,9 @@
         <v>21.73</v>
       </c>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B53">
         <v>78.3</v>
@@ -4637,10 +4639,10 @@
         <v>113.63</v>
       </c>
       <c r="D53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F53">
         <v>114.13</v>
@@ -4652,19 +4654,19 @@
         <v>112.14</v>
       </c>
       <c r="I53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J53">
         <v>112.97</v>
       </c>
       <c r="K53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L53">
         <v>110.99</v>
       </c>
       <c r="M53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N53">
         <v>108.86</v>
@@ -4685,13 +4687,13 @@
         <v>113.97</v>
       </c>
       <c r="T53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U53">
         <v>111.98</v>
       </c>
       <c r="V53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W53">
         <v>113.8</v>
@@ -4718,9 +4720,9 @@
         <v>21.73</v>
       </c>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B54">
         <v>80.3</v>
@@ -4729,10 +4731,10 @@
         <v>112.97</v>
       </c>
       <c r="D54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F54">
         <v>113.8</v>
@@ -4744,19 +4746,19 @@
         <v>111.98</v>
       </c>
       <c r="I54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J54">
         <v>112.64</v>
       </c>
       <c r="K54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L54">
         <v>110.99</v>
       </c>
       <c r="M54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N54">
         <v>108.69</v>
@@ -4777,13 +4779,13 @@
         <v>113.8</v>
       </c>
       <c r="T54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U54">
         <v>112.14</v>
       </c>
       <c r="V54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W54">
         <v>113.63</v>
@@ -4810,9 +4812,9 @@
         <v>21.73</v>
       </c>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B55">
         <v>82.32</v>
@@ -4821,10 +4823,10 @@
         <v>113.14</v>
       </c>
       <c r="D55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F55">
         <v>113.63</v>
@@ -4836,19 +4838,19 @@
         <v>111.98</v>
       </c>
       <c r="I55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J55">
         <v>112.97</v>
       </c>
       <c r="K55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L55">
         <v>110.99</v>
       </c>
       <c r="M55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N55">
         <v>108.86</v>
@@ -4869,13 +4871,13 @@
         <v>113.8</v>
       </c>
       <c r="T55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U55">
         <v>111.81</v>
       </c>
       <c r="V55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W55">
         <v>113.47</v>
@@ -4902,9 +4904,9 @@
         <v>21.72</v>
       </c>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B56">
         <v>84.32</v>
@@ -4913,10 +4915,10 @@
         <v>112.97</v>
       </c>
       <c r="D56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F56">
         <v>113.8</v>
@@ -4928,19 +4930,19 @@
         <v>111.32</v>
       </c>
       <c r="I56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J56">
         <v>112.31</v>
       </c>
       <c r="K56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L56">
         <v>110.83</v>
       </c>
       <c r="M56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N56">
         <v>108.69</v>
@@ -4961,13 +4963,13 @@
         <v>113.63</v>
       </c>
       <c r="T56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U56">
         <v>111.98</v>
       </c>
       <c r="V56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W56">
         <v>113.47</v>
@@ -4994,9 +4996,9 @@
         <v>21.72</v>
       </c>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B57">
         <v>86.32</v>
@@ -5005,10 +5007,10 @@
         <v>112.81</v>
       </c>
       <c r="D57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F57">
         <v>113.63</v>
@@ -5020,19 +5022,19 @@
         <v>111.32</v>
       </c>
       <c r="I57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J57">
         <v>112.14</v>
       </c>
       <c r="K57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L57">
         <v>110.99</v>
       </c>
       <c r="M57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N57">
         <v>108.69</v>
@@ -5053,13 +5055,13 @@
         <v>113.47</v>
       </c>
       <c r="T57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U57">
         <v>111.98</v>
       </c>
       <c r="V57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W57">
         <v>113.47</v>
@@ -5086,9 +5088,9 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B58">
         <v>88.32</v>
@@ -5097,10 +5099,10 @@
         <v>112.64</v>
       </c>
       <c r="D58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F58">
         <v>113.47</v>
@@ -5112,19 +5114,19 @@
         <v>111.16</v>
       </c>
       <c r="I58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J58">
         <v>112.31</v>
       </c>
       <c r="K58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L58">
         <v>110.66</v>
       </c>
       <c r="M58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N58">
         <v>108.53</v>
@@ -5145,13 +5147,13 @@
         <v>113.47</v>
       </c>
       <c r="T58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U58">
         <v>111.65</v>
       </c>
       <c r="V58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W58">
         <v>113.47</v>
@@ -5178,9 +5180,9 @@
         <v>21.72</v>
       </c>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B59">
         <v>90.32</v>
@@ -5189,10 +5191,10 @@
         <v>112.47</v>
       </c>
       <c r="D59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F59">
         <v>113.14</v>
@@ -5204,19 +5206,19 @@
         <v>111.16</v>
       </c>
       <c r="I59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J59">
         <v>112.47</v>
       </c>
       <c r="K59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L59">
         <v>110.66</v>
       </c>
       <c r="M59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N59">
         <v>108.2</v>
@@ -5237,13 +5239,13 @@
         <v>112.97</v>
       </c>
       <c r="T59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U59">
         <v>111.65</v>
       </c>
       <c r="V59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W59">
         <v>113.3</v>
@@ -5270,9 +5272,9 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B60">
         <v>92.33</v>
@@ -5281,10 +5283,10 @@
         <v>112.64</v>
       </c>
       <c r="D60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F60">
         <v>112.97</v>
@@ -5296,19 +5298,19 @@
         <v>110.99</v>
       </c>
       <c r="I60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J60">
         <v>111.81</v>
       </c>
       <c r="K60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L60">
         <v>111.16</v>
       </c>
       <c r="M60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N60">
         <v>108.2</v>
@@ -5329,13 +5331,13 @@
         <v>113.3</v>
       </c>
       <c r="T60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U60">
         <v>111.32</v>
       </c>
       <c r="V60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W60">
         <v>113.3</v>
@@ -5362,9 +5364,9 @@
         <v>21.72</v>
       </c>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B61">
         <v>94.33</v>
@@ -5373,10 +5375,10 @@
         <v>112.64</v>
       </c>
       <c r="D61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F61">
         <v>112.97</v>
@@ -5388,19 +5390,19 @@
         <v>110.99</v>
       </c>
       <c r="I61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J61">
         <v>111.65</v>
       </c>
       <c r="K61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L61">
         <v>110.66</v>
       </c>
       <c r="M61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N61">
         <v>107.71</v>
@@ -5421,13 +5423,13 @@
         <v>113.63</v>
       </c>
       <c r="T61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U61">
         <v>111.32</v>
       </c>
       <c r="V61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W61">
         <v>113.3</v>
@@ -5454,9 +5456,9 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B62">
         <v>96.33</v>
@@ -5465,10 +5467,10 @@
         <v>112.31</v>
       </c>
       <c r="D62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F62">
         <v>112.97</v>
@@ -5480,19 +5482,19 @@
         <v>110.83</v>
       </c>
       <c r="I62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J62">
         <v>111.65</v>
       </c>
       <c r="K62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L62">
         <v>110.5</v>
       </c>
       <c r="M62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N62">
         <v>107.88</v>
@@ -5513,13 +5515,13 @@
         <v>113.3</v>
       </c>
       <c r="T62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U62">
         <v>110.99</v>
       </c>
       <c r="V62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W62">
         <v>113.14</v>
@@ -5546,9 +5548,9 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B63">
         <v>98.33</v>
@@ -5557,10 +5559,10 @@
         <v>112.31</v>
       </c>
       <c r="D63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F63">
         <v>113.3</v>
@@ -5572,19 +5574,19 @@
         <v>111.16</v>
       </c>
       <c r="I63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J63">
         <v>111.65</v>
       </c>
       <c r="K63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L63">
         <v>110</v>
       </c>
       <c r="M63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N63">
         <v>107.71</v>
@@ -5605,13 +5607,13 @@
         <v>112.81</v>
       </c>
       <c r="T63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U63">
         <v>111.48</v>
       </c>
       <c r="V63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W63">
         <v>113.14</v>
@@ -5638,9 +5640,9 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B64">
         <v>100.35</v>
@@ -5649,10 +5651,10 @@
         <v>112.14</v>
       </c>
       <c r="D64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F64">
         <v>112.81</v>
@@ -5664,19 +5666,19 @@
         <v>110.66</v>
       </c>
       <c r="I64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J64">
         <v>111.48</v>
       </c>
       <c r="K64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L64">
         <v>110</v>
       </c>
       <c r="M64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N64">
         <v>107.55</v>
@@ -5697,13 +5699,13 @@
         <v>112.81</v>
       </c>
       <c r="T64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U64">
         <v>110.99</v>
       </c>
       <c r="V64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W64">
         <v>113.14</v>
@@ -5730,9 +5732,9 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B65">
         <v>102.35</v>
@@ -5741,10 +5743,10 @@
         <v>111.98</v>
       </c>
       <c r="D65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F65">
         <v>112.81</v>
@@ -5756,19 +5758,19 @@
         <v>110.5</v>
       </c>
       <c r="I65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J65">
         <v>111.32</v>
       </c>
       <c r="K65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L65">
         <v>109.84</v>
       </c>
       <c r="M65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N65">
         <v>107.39</v>
@@ -5789,13 +5791,13 @@
         <v>112.47</v>
       </c>
       <c r="T65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U65">
         <v>110.83</v>
       </c>
       <c r="V65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W65">
         <v>112.81</v>
@@ -5822,9 +5824,9 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B66">
         <v>104.35</v>
@@ -5833,10 +5835,10 @@
         <v>111.48</v>
       </c>
       <c r="D66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F66">
         <v>112.47</v>
@@ -5848,19 +5850,19 @@
         <v>110.33</v>
       </c>
       <c r="I66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J66">
         <v>110.83</v>
       </c>
       <c r="K66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L66">
         <v>109.84</v>
       </c>
       <c r="M66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N66">
         <v>107.23</v>
@@ -5881,13 +5883,13 @@
         <v>112.47</v>
       </c>
       <c r="T66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U66">
         <v>110.83</v>
       </c>
       <c r="V66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W66">
         <v>112.97</v>
@@ -5914,9 +5916,9 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B67">
         <v>106.35</v>
@@ -5925,10 +5927,10 @@
         <v>111.48</v>
       </c>
       <c r="D67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F67">
         <v>112.64</v>
@@ -5940,19 +5942,19 @@
         <v>110.5</v>
       </c>
       <c r="I67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J67">
         <v>110.66</v>
       </c>
       <c r="K67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L67">
         <v>109.84</v>
       </c>
       <c r="M67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N67">
         <v>106.9</v>
@@ -5973,13 +5975,13 @@
         <v>112.64</v>
       </c>
       <c r="T67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U67">
         <v>110.66</v>
       </c>
       <c r="V67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W67">
         <v>112.64</v>
@@ -6006,9 +6008,9 @@
         <v>21.68</v>
       </c>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B68">
         <v>108.35</v>
@@ -6017,10 +6019,10 @@
         <v>111.48</v>
       </c>
       <c r="D68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F68">
         <v>112.64</v>
@@ -6032,19 +6034,19 @@
         <v>110</v>
       </c>
       <c r="I68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J68">
         <v>110.99</v>
       </c>
       <c r="K68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L68">
         <v>109.35</v>
       </c>
       <c r="M68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N68">
         <v>106.9</v>
@@ -6065,13 +6067,13 @@
         <v>112.47</v>
       </c>
       <c r="T68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U68">
         <v>110.83</v>
       </c>
       <c r="V68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W68">
         <v>112.97</v>
@@ -6098,9 +6100,9 @@
         <v>21.68</v>
       </c>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B69">
         <v>110.37</v>
@@ -6109,10 +6111,10 @@
         <v>111.16</v>
       </c>
       <c r="D69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F69">
         <v>112.81</v>
@@ -6124,19 +6126,19 @@
         <v>110.17</v>
       </c>
       <c r="I69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J69">
         <v>110.83</v>
       </c>
       <c r="K69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L69">
         <v>109.84</v>
       </c>
       <c r="M69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N69">
         <v>106.57</v>
@@ -6157,13 +6159,13 @@
         <v>112.47</v>
       </c>
       <c r="T69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U69">
         <v>110.5</v>
       </c>
       <c r="V69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W69">
         <v>112.81</v>
@@ -6190,9 +6192,9 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B70">
         <v>112.37</v>
@@ -6201,10 +6203,10 @@
         <v>111.32</v>
       </c>
       <c r="D70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F70">
         <v>112.31</v>
@@ -6216,19 +6218,19 @@
         <v>109.68</v>
       </c>
       <c r="I70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J70">
         <v>110.66</v>
       </c>
       <c r="K70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L70">
         <v>109.35</v>
       </c>
       <c r="M70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N70">
         <v>106.74</v>
@@ -6249,13 +6251,13 @@
         <v>112.31</v>
       </c>
       <c r="T70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U70">
         <v>110.83</v>
       </c>
       <c r="V70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W70">
         <v>112.81</v>
@@ -6282,9 +6284,9 @@
         <v>21.68</v>
       </c>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B71">
         <v>114.37</v>
@@ -6293,10 +6295,10 @@
         <v>110.99</v>
       </c>
       <c r="D71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F71">
         <v>112.31</v>
@@ -6308,19 +6310,19 @@
         <v>109.51</v>
       </c>
       <c r="I71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J71">
         <v>110.66</v>
       </c>
       <c r="K71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L71">
         <v>109.35</v>
       </c>
       <c r="M71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N71">
         <v>106.74</v>
@@ -6341,13 +6343,13 @@
         <v>111.98</v>
       </c>
       <c r="T71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U71">
         <v>110.33</v>
       </c>
       <c r="V71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W71">
         <v>112.47</v>
@@ -6374,9 +6376,9 @@
         <v>21.68</v>
       </c>
     </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B72">
         <v>116.37</v>
@@ -6385,10 +6387,10 @@
         <v>111.16</v>
       </c>
       <c r="D72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F72">
         <v>112.47</v>
@@ -6400,19 +6402,19 @@
         <v>109.35</v>
       </c>
       <c r="I72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J72">
         <v>110.99</v>
       </c>
       <c r="K72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L72">
         <v>109.51</v>
       </c>
       <c r="M72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N72">
         <v>106.57</v>
@@ -6433,13 +6435,13 @@
         <v>112.14</v>
       </c>
       <c r="T72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U72">
         <v>110.33</v>
       </c>
       <c r="V72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W72">
         <v>112.64</v>
@@ -6466,9 +6468,9 @@
         <v>21.68</v>
       </c>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B73">
         <v>118.37</v>
@@ -6477,10 +6479,10 @@
         <v>111.16</v>
       </c>
       <c r="D73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F73">
         <v>112.31</v>
@@ -6492,19 +6494,19 @@
         <v>109.19</v>
       </c>
       <c r="I73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J73">
         <v>110.17</v>
       </c>
       <c r="K73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L73">
         <v>109.51</v>
       </c>
       <c r="M73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N73">
         <v>106.74</v>
@@ -6525,13 +6527,13 @@
         <v>112.14</v>
       </c>
       <c r="T73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U73">
         <v>110.17</v>
       </c>
       <c r="V73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W73">
         <v>112.47</v>
@@ -6558,9 +6560,9 @@
         <v>21.68</v>
       </c>
     </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B74">
         <v>120.38</v>
@@ -6569,10 +6571,10 @@
         <v>110.99</v>
       </c>
       <c r="D74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F74">
         <v>112.31</v>
@@ -6584,19 +6586,19 @@
         <v>108.86</v>
       </c>
       <c r="I74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J74">
         <v>110.17</v>
       </c>
       <c r="K74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L74">
         <v>109.51</v>
       </c>
       <c r="M74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N74">
         <v>106.09</v>
@@ -6617,13 +6619,13 @@
         <v>112.14</v>
       </c>
       <c r="T74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U74">
         <v>110.17</v>
       </c>
       <c r="V74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W74">
         <v>112.47</v>
@@ -6650,9 +6652,9 @@
         <v>21.68</v>
       </c>
     </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B75">
         <v>122.38</v>
@@ -6661,10 +6663,10 @@
         <v>110.66</v>
       </c>
       <c r="D75" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E75" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F75">
         <v>112.14</v>
@@ -6676,19 +6678,19 @@
         <v>109.02</v>
       </c>
       <c r="I75" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J75">
         <v>109.84</v>
       </c>
       <c r="K75" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L75">
         <v>109.35</v>
       </c>
       <c r="M75" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N75">
         <v>106.25</v>
@@ -6709,13 +6711,13 @@
         <v>111.81</v>
       </c>
       <c r="T75" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U75">
         <v>109.84</v>
       </c>
       <c r="V75" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W75">
         <v>112.31</v>
@@ -6742,9 +6744,9 @@
         <v>21.68</v>
       </c>
     </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B76">
         <v>124.38</v>
@@ -6753,10 +6755,10 @@
         <v>110.66</v>
       </c>
       <c r="D76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F76">
         <v>112.14</v>
@@ -6768,19 +6770,19 @@
         <v>108.69</v>
       </c>
       <c r="I76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J76">
         <v>109.51</v>
       </c>
       <c r="K76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L76">
         <v>109.35</v>
       </c>
       <c r="M76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N76">
         <v>106.57</v>
@@ -6801,13 +6803,13 @@
         <v>111.48</v>
       </c>
       <c r="T76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U76">
         <v>110</v>
       </c>
       <c r="V76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W76">
         <v>112.14</v>
@@ -6834,9 +6836,9 @@
         <v>21.67</v>
       </c>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B77">
         <v>126.38</v>
@@ -6845,10 +6847,10 @@
         <v>110.5</v>
       </c>
       <c r="D77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F77">
         <v>111.81</v>
@@ -6860,19 +6862,19 @@
         <v>109.02</v>
       </c>
       <c r="I77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J77">
         <v>109.84</v>
       </c>
       <c r="K77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L77">
         <v>109.02</v>
       </c>
       <c r="M77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N77">
         <v>106.09</v>
@@ -6893,13 +6895,13 @@
         <v>111.48</v>
       </c>
       <c r="T77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U77">
         <v>110</v>
       </c>
       <c r="V77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W77">
         <v>112.31</v>
@@ -6926,9 +6928,9 @@
         <v>21.68</v>
       </c>
     </row>
-    <row r="78" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B78">
         <v>128.38</v>
@@ -6937,10 +6939,10 @@
         <v>110.17</v>
       </c>
       <c r="D78" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E78" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F78">
         <v>111.81</v>
@@ -6952,19 +6954,19 @@
         <v>108.69</v>
       </c>
       <c r="I78" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J78">
         <v>109.35</v>
       </c>
       <c r="K78" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L78">
         <v>109.35</v>
       </c>
       <c r="M78" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N78">
         <v>106.09</v>
@@ -6985,13 +6987,13 @@
         <v>111.65</v>
       </c>
       <c r="T78" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U78">
         <v>109.84</v>
       </c>
       <c r="V78" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W78">
         <v>112.47</v>
@@ -7018,9 +7020,9 @@
         <v>21.68</v>
       </c>
     </row>
-    <row r="79" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B79">
         <v>130.38</v>
@@ -7029,10 +7031,10 @@
         <v>110.33</v>
       </c>
       <c r="D79" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E79" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F79">
         <v>111.98</v>
@@ -7044,19 +7046,19 @@
         <v>108.37</v>
       </c>
       <c r="I79" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J79">
         <v>109.68</v>
       </c>
       <c r="K79" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L79">
         <v>109.51</v>
       </c>
       <c r="M79" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N79">
         <v>105.76</v>
@@ -7077,13 +7079,13 @@
         <v>111.48</v>
       </c>
       <c r="T79" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U79">
         <v>109.84</v>
       </c>
       <c r="V79" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W79">
         <v>112.31</v>
@@ -7110,9 +7112,9 @@
         <v>21.68</v>
       </c>
     </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B80">
         <v>132.38</v>
@@ -7121,10 +7123,10 @@
         <v>110.33</v>
       </c>
       <c r="D80" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E80" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F80">
         <v>111.65</v>
@@ -7136,19 +7138,19 @@
         <v>108.37</v>
       </c>
       <c r="I80" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J80">
         <v>109.51</v>
       </c>
       <c r="K80" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L80">
         <v>109.02</v>
       </c>
       <c r="M80" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N80">
         <v>105.93</v>
@@ -7169,13 +7171,13 @@
         <v>111.65</v>
       </c>
       <c r="T80" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U80">
         <v>109.84</v>
       </c>
       <c r="V80" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W80">
         <v>112.31</v>
@@ -7202,9 +7204,9 @@
         <v>21.68</v>
       </c>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B81">
         <v>134.4</v>
@@ -7213,10 +7215,10 @@
         <v>110.17</v>
       </c>
       <c r="D81" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E81" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F81">
         <v>111.81</v>
@@ -7228,19 +7230,19 @@
         <v>108.2</v>
       </c>
       <c r="I81" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J81">
         <v>108.69</v>
       </c>
       <c r="K81" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L81">
         <v>109.02</v>
       </c>
       <c r="M81" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N81">
         <v>105.93</v>
@@ -7261,13 +7263,13 @@
         <v>111.81</v>
       </c>
       <c r="T81" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U81">
         <v>109.68</v>
       </c>
       <c r="V81" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W81">
         <v>112.31</v>
@@ -7294,9 +7296,9 @@
         <v>21.68</v>
       </c>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B82">
         <v>136.41999999999999</v>
@@ -7305,10 +7307,10 @@
         <v>110</v>
       </c>
       <c r="D82" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E82" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F82">
         <v>111.81</v>
@@ -7320,19 +7322,19 @@
         <v>108.37</v>
       </c>
       <c r="I82" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J82">
         <v>108.86</v>
       </c>
       <c r="K82" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L82">
         <v>108.86</v>
       </c>
       <c r="M82" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N82">
         <v>105.76</v>
@@ -7353,13 +7355,13 @@
         <v>111.48</v>
       </c>
       <c r="T82" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U82">
         <v>109.51</v>
       </c>
       <c r="V82" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W82">
         <v>112.47</v>
@@ -7386,9 +7388,9 @@
         <v>21.68</v>
       </c>
     </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B83">
         <v>138.41999999999999</v>
@@ -7397,10 +7399,10 @@
         <v>109.68</v>
       </c>
       <c r="D83" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E83" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F83">
         <v>111.65</v>
@@ -7412,19 +7414,19 @@
         <v>108.04</v>
       </c>
       <c r="I83" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J83">
         <v>108.53</v>
       </c>
       <c r="K83" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L83">
         <v>108.86</v>
       </c>
       <c r="M83" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N83">
         <v>105.6</v>
@@ -7445,13 +7447,13 @@
         <v>111.48</v>
       </c>
       <c r="T83" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U83">
         <v>109.51</v>
       </c>
       <c r="V83" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W83">
         <v>112.47</v>
@@ -7478,9 +7480,9 @@
         <v>21.68</v>
       </c>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B84">
         <v>140.43</v>
@@ -7489,10 +7491,10 @@
         <v>109.68</v>
       </c>
       <c r="D84" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E84" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F84">
         <v>111.65</v>
@@ -7504,19 +7506,19 @@
         <v>108.2</v>
       </c>
       <c r="I84" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J84">
         <v>108.37</v>
       </c>
       <c r="K84" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L84">
         <v>108.69</v>
       </c>
       <c r="M84" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N84">
         <v>105.28</v>
@@ -7537,13 +7539,13 @@
         <v>111.32</v>
       </c>
       <c r="T84" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U84">
         <v>109.51</v>
       </c>
       <c r="V84" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W84">
         <v>112.14</v>
@@ -7570,9 +7572,9 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="85" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B85">
         <v>142.44999999999999</v>
@@ -7581,10 +7583,10 @@
         <v>109.68</v>
       </c>
       <c r="D85" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E85" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F85">
         <v>111.32</v>
@@ -7596,19 +7598,19 @@
         <v>107.88</v>
       </c>
       <c r="I85" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J85">
         <v>108.37</v>
       </c>
       <c r="K85" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L85">
         <v>108.86</v>
       </c>
       <c r="M85" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N85">
         <v>105.28</v>
@@ -7629,13 +7631,13 @@
         <v>110.99</v>
       </c>
       <c r="T85" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U85">
         <v>109.35</v>
       </c>
       <c r="V85" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W85">
         <v>112.14</v>
@@ -7673,7 +7675,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>